<commit_message>
Added example EAN and UPC barcodes
Signed-off-by: Rlisbona <rlisbona@smu.edu>
</commit_message>
<xml_diff>
--- a/Explore/GTIN Tables And Record Counts.xlsx
+++ b/Explore/GTIN Tables And Record Counts.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="17160" windowHeight="27135"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="17160" windowHeight="21840"/>
   </bookViews>
   <sheets>
     <sheet name="GTIN Tables And Record Counts" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -85,7 +85,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -224,7 +224,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -410,8 +410,50 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FF66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -526,6 +568,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -572,10 +629,25 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="34" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="38" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="35" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="37" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="36" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="39" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="40" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -652,6 +724,17 @@
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
+  <colors>
+    <mruColors>
+      <color rgb="FF66FFFF"/>
+      <color rgb="FFFFFF99"/>
+      <color rgb="FFCCCCFF"/>
+      <color rgb="FF9999FF"/>
+      <color rgb="FFFFCC99"/>
+      <color rgb="FFCCFF99"/>
+      <color rgb="FF66FF66"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -947,26 +1030,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection sqref="A1:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -980,10 +1063,10 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="5">
         <v>4151</v>
       </c>
       <c r="C2" s="1">
@@ -997,14 +1080,14 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1">
-        <v>3</v>
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="5">
+        <v>32</v>
       </c>
       <c r="C3" s="1">
-        <v>5461</v>
+        <v>512</v>
       </c>
       <c r="D3" s="1">
         <v>16384</v>
@@ -1014,82 +1097,82 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1">
-        <v>32</v>
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="5">
+        <v>581</v>
       </c>
       <c r="C4" s="1">
-        <v>512</v>
+        <v>84</v>
       </c>
       <c r="D4" s="1">
+        <v>49152</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>8192</v>
+      </c>
+      <c r="D5" s="1">
         <v>16384</v>
       </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1">
-        <v>581</v>
-      </c>
-      <c r="C5" s="1">
-        <v>84</v>
-      </c>
-      <c r="D5" s="1">
-        <v>49152</v>
-      </c>
       <c r="E5" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1">
-        <v>2</v>
+      <c r="A6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="7">
+        <v>1549550</v>
       </c>
       <c r="C6" s="1">
-        <v>8192</v>
+        <v>123</v>
       </c>
       <c r="D6" s="1">
+        <v>191610880</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="7">
+        <v>264</v>
+      </c>
+      <c r="C7" s="1">
+        <v>62</v>
+      </c>
+      <c r="D7" s="1">
         <v>16384</v>
       </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1549550</v>
-      </c>
-      <c r="C7" s="1">
-        <v>123</v>
-      </c>
-      <c r="D7" s="1">
-        <v>191610880</v>
-      </c>
       <c r="E7" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="1">
-        <v>264</v>
+      <c r="A8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="7">
+        <v>16</v>
       </c>
       <c r="C8" s="1">
-        <v>62</v>
+        <v>1024</v>
       </c>
       <c r="D8" s="1">
         <v>16384</v>
@@ -1099,155 +1182,159 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="1">
+      <c r="A9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="9">
+        <v>38760</v>
+      </c>
+      <c r="C9" s="1">
+        <v>122</v>
+      </c>
+      <c r="D9" s="1">
+        <v>4734976</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="9">
+        <v>3298</v>
+      </c>
+      <c r="C10" s="1">
+        <v>69</v>
+      </c>
+      <c r="D10" s="1">
+        <v>229376</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="11">
+        <v>1000</v>
+      </c>
+      <c r="C11" s="1">
+        <v>81</v>
+      </c>
+      <c r="D11" s="1">
+        <v>81920</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="1">
-        <v>1024</v>
-      </c>
-      <c r="D9" s="1">
-        <v>16384</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="1">
-        <v>38760</v>
-      </c>
-      <c r="C10" s="1">
-        <v>122</v>
-      </c>
-      <c r="D10" s="1">
-        <v>4734976</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="1">
-        <v>3298</v>
-      </c>
-      <c r="C11" s="1">
-        <v>69</v>
-      </c>
-      <c r="D11" s="1">
-        <v>229376</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="1">
-        <v>1000</v>
+      <c r="B12" s="13">
+        <v>844270</v>
       </c>
       <c r="C12" s="1">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="D12" s="1">
-        <v>81920</v>
+        <v>89833472</v>
       </c>
       <c r="E12" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="1">
-        <v>844270</v>
+      <c r="A13" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="15">
+        <v>231</v>
       </c>
       <c r="C13" s="1">
-        <v>106</v>
+        <v>638</v>
       </c>
       <c r="D13" s="1">
-        <v>89833472</v>
+        <v>147456</v>
       </c>
       <c r="E13" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="1">
-        <v>2</v>
+      <c r="A14" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="17">
+        <v>42</v>
       </c>
       <c r="C14" s="1">
-        <v>8192</v>
+        <v>390</v>
       </c>
       <c r="D14" s="1">
         <v>16384</v>
       </c>
       <c r="E14" s="1">
-        <v>0</v>
+        <v>16384</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1">
+        <v>8192</v>
+      </c>
+      <c r="D20" s="1">
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B21" s="1">
         <v>3</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C21" s="1">
         <v>5461</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D21" s="1">
         <v>16384</v>
       </c>
-      <c r="E15" s="1">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="1">
+        <v>3</v>
+      </c>
+      <c r="C26" s="1">
+        <v>5461</v>
+      </c>
+      <c r="D26" s="1">
         <v>16384</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="1">
-        <v>231</v>
-      </c>
-      <c r="C16" s="1">
-        <v>638</v>
-      </c>
-      <c r="D16" s="1">
-        <v>147456</v>
-      </c>
-      <c r="E16" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="1">
-        <v>42</v>
-      </c>
-      <c r="C17" s="1">
-        <v>390</v>
-      </c>
-      <c r="D17" s="1">
-        <v>16384</v>
-      </c>
-      <c r="E17" s="1">
+      <c r="E26" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Created presentation, updated SQL with coded needed for slides
</commit_message>
<xml_diff>
--- a/Explore/GTIN Tables And Record Counts.xlsx
+++ b/Explore/GTIN Tables And Record Counts.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
   <si>
     <t>TABLE_NAME</t>
   </si>
@@ -629,7 +629,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -648,6 +648,9 @@
     <xf numFmtId="164" fontId="0" fillId="39" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="40" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1030,22 +1033,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B14"/>
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.140625" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1062,7 +1067,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1078,8 +1083,18 @@
       <c r="E2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H2" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="18">
+        <v>4</v>
+      </c>
+      <c r="J2">
+        <f>+I2*B2</f>
+        <v>16604</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -1095,8 +1110,20 @@
       <c r="E3" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H3" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="18">
+        <v>4</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J14" si="0">+I3*B3</f>
+        <v>128</v>
+      </c>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -1112,8 +1139,18 @@
       <c r="E4" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H4" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="18">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -1129,8 +1166,18 @@
       <c r="E5" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H5" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="18">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
@@ -1146,8 +1193,20 @@
       <c r="E6" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H6" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="18">
+        <v>23</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>35639650</v>
+      </c>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>11</v>
       </c>
@@ -1163,8 +1222,18 @@
       <c r="E7" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H7" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="18">
+        <v>3</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>792</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -1180,8 +1249,18 @@
       <c r="E8" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H8" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="18">
+        <v>3</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>13</v>
       </c>
@@ -1197,8 +1276,18 @@
       <c r="E9" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H9" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="18">
+        <v>5</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>193800</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>14</v>
       </c>
@@ -1214,8 +1303,20 @@
       <c r="E10" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H10" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="18">
+        <v>4</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>13192</v>
+      </c>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>15</v>
       </c>
@@ -1231,8 +1332,18 @@
       <c r="E11" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H11" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="18">
+        <v>3</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>16</v>
       </c>
@@ -1248,8 +1359,18 @@
       <c r="E12" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H12" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="18">
+        <v>21</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>17729670</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>19</v>
       </c>
@@ -1265,8 +1386,20 @@
       <c r="E13" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H13" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="18">
+        <v>30</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>6930</v>
+      </c>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>20</v>
       </c>
@@ -1282,16 +1415,34 @@
       <c r="E14" s="1">
         <v>16384</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H14" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="18">
+        <v>3</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E15" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <f>SUM(J2:J14)</f>
+        <v>53605106</v>
+      </c>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E16" s="1">
         <v>0</v>
       </c>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">

</xml_diff>